<commit_message>
Updated QA-eval scores and KG statistics
</commit_message>
<xml_diff>
--- a/Evaluation/result/KG_eval/correctness-comprehensiveness_all-scores.xlsx
+++ b/Evaluation/result/KG_eval/correctness-comprehensiveness_all-scores.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huyen\OneDrive\Documents\GitHub\CORD-19-KG\Evaluation\result\KG_eval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A486FF9E-6F65-4C1D-9ABB-B7A6473989ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4559D061-A0B1-4947-A272-55F7AA6B5C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{472E2F60-D8EA-434C-9462-E3C74449F5E0}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{472E2F60-D8EA-434C-9462-E3C74449F5E0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="result_old" sheetId="1" r:id="rId1"/>
+    <sheet name="result_new" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>subset_1</t>
   </si>
@@ -92,6 +93,12 @@
   </si>
   <si>
     <t>treat-procedure</t>
+  </si>
+  <si>
+    <t>avg_relatedness</t>
+  </si>
+  <si>
+    <t>avg_correctness</t>
   </si>
 </sst>
 </file>
@@ -99,7 +106,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -132,7 +139,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,19 +454,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9DD0127-0FD9-4F16-A3B3-A63B474A4418}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.7265625" customWidth="1"/>
+    <col min="2" max="2" width="16.08984375" customWidth="1"/>
     <col min="3" max="10" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>10</v>
       </c>
@@ -487,328 +494,1076 @@
       <c r="J1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>0.41085271317829403</v>
+        <v>0.41099999999999998</v>
       </c>
       <c r="C2" s="1">
-        <v>0.64174735419950402</v>
+        <v>0.64200000000000002</v>
       </c>
       <c r="D2" s="1">
-        <v>0.61686557081738302</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="E2" s="1">
-        <v>0.64913459922701999</v>
+        <v>0.64900000000000002</v>
       </c>
       <c r="F2" s="1">
-        <v>7.9806529625151099E-2</v>
+        <v>0.08</v>
       </c>
       <c r="G2" s="1">
-        <v>5.2915766738660899E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="H2" s="1">
-        <v>0.70172724929105401</v>
+        <v>0.70199999999999996</v>
       </c>
       <c r="I2" s="1">
-        <v>0.59487179487179398</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="J2" s="1">
-        <v>0.31191037735848998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>0.312</v>
+      </c>
+      <c r="K2" s="1">
+        <f>SUM(E2:J2)/COUNT(E2:J2)</f>
+        <v>0.39849999999999991</v>
+      </c>
+      <c r="L2" t="str">
+        <f>_xlfn.TEXTJOIN(" &amp; ", FALSE, A2:J2)</f>
+        <v>subset_1 &amp; 0.411 &amp; 0.642 &amp; 0.617 &amp; 0.649 &amp; 0.08 &amp; 0.053 &amp; 0.702 &amp; 0.595 &amp; 0.312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>0.434108527131782</v>
+        <v>0.434</v>
       </c>
       <c r="C3" s="1">
-        <v>0.64914996622382304</v>
+        <v>0.64900000000000002</v>
       </c>
       <c r="D3" s="1">
-        <v>0.61495158748029699</v>
+        <v>0.61499999999999999</v>
       </c>
       <c r="E3" s="1">
-        <v>0.64535585042219501</v>
+        <v>0.64500000000000002</v>
       </c>
       <c r="F3" s="1">
-        <v>8.4601339013998703E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="G3" s="1">
-        <v>5.6302939711011399E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="H3" s="1">
-        <v>0.71552579365079305</v>
+        <v>0.71599999999999997</v>
       </c>
       <c r="I3" s="1">
-        <v>0.58602150537634401</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="J3" s="1">
-        <v>0.293944738389182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" ref="K3:K11" si="0">SUM(E3:J3)/COUNT(E3:J3)</f>
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L11" si="1">_xlfn.TEXTJOIN(" &amp; ", FALSE, A3:J3)</f>
+        <v>subset_2 &amp; 0.434 &amp; 0.649 &amp; 0.615 &amp; 0.645 &amp; 0.085 &amp; 0.056 &amp; 0.716 &amp; 0.586 &amp; 0.294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>0.44186046511627902</v>
+        <v>0.442</v>
       </c>
       <c r="C4" s="1">
-        <v>0.65750956991668497</v>
+        <v>0.65800000000000003</v>
       </c>
       <c r="D4" s="1">
-        <v>0.63694363131426801</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="E4" s="1">
-        <v>0.66195920197265101</v>
+        <v>0.66200000000000003</v>
       </c>
       <c r="F4" s="1">
-        <v>0.11632415664986399</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="G4" s="1">
-        <v>6.2521008403361306E-2</v>
+        <v>6.3E-2</v>
       </c>
       <c r="H4" s="1">
-        <v>0.70240472263217202</v>
+        <v>0.70199999999999996</v>
       </c>
       <c r="I4" s="1">
-        <v>0.56208053691275095</v>
+        <v>0.56200000000000006</v>
       </c>
       <c r="J4" s="1">
-        <v>0.29901558654634902</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.40066666666666667</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="1"/>
+        <v>subset_3 &amp; 0.442 &amp; 0.658 &amp; 0.637 &amp; 0.662 &amp; 0.116 &amp; 0.063 &amp; 0.702 &amp; 0.562 &amp; 0.299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>0.46511627906976699</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="C5" s="1">
-        <v>0.65514523755910803</v>
+        <v>0.65500000000000003</v>
       </c>
       <c r="D5" s="1">
-        <v>0.63437288898896604</v>
+        <v>0.63400000000000001</v>
       </c>
       <c r="E5" s="1">
-        <v>0.67014631641995304</v>
+        <v>0.67</v>
       </c>
       <c r="F5" s="1">
-        <v>0.11503067484662501</v>
+        <v>0.115</v>
       </c>
       <c r="G5" s="1">
-        <v>6.3844880586426997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="H5" s="1">
-        <v>0.69543973941367998</v>
+        <v>0.69499999999999995</v>
       </c>
       <c r="I5" s="1">
-        <v>0.63403944485025499</v>
+        <v>0.63400000000000001</v>
       </c>
       <c r="J5" s="1">
-        <v>0.30467122880095199</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.41383333333333333</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="1"/>
+        <v>subset_4 &amp; 0.465 &amp; 0.655 &amp; 0.634 &amp; 0.67 &amp; 0.115 &amp; 0.064 &amp; 0.695 &amp; 0.634 &amp; 0.305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>0.49612403100775099</v>
+        <v>0.496</v>
       </c>
       <c r="C6" s="1">
-        <v>0.65204908804323303</v>
+        <v>0.65200000000000002</v>
       </c>
       <c r="D6" s="1">
-        <v>0.62690835397432998</v>
+        <v>0.627</v>
       </c>
       <c r="E6" s="1">
-        <v>0.67264356675551196</v>
+        <v>0.67300000000000004</v>
       </c>
       <c r="F6" s="1">
-        <v>0.10841086007214699</v>
+        <v>0.108</v>
       </c>
       <c r="G6" s="1">
-        <v>6.2345896442409302E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="H6" s="1">
-        <v>0.69323131911091196</v>
+        <v>0.69299999999999995</v>
       </c>
       <c r="I6" s="1">
-        <v>0.64501953125</v>
+        <v>0.64500000000000002</v>
       </c>
       <c r="J6" s="1">
-        <v>0.31571722717913497</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+        <v>0.316</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.41616666666666663</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="1"/>
+        <v>subset_5 &amp; 0.496 &amp; 0.652 &amp; 0.627 &amp; 0.673 &amp; 0.108 &amp; 0.062 &amp; 0.693 &amp; 0.645 &amp; 0.316</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>0.49612403100775099</v>
+        <v>0.496</v>
       </c>
       <c r="C7" s="1">
-        <v>0.65125443320635701</v>
+        <v>0.65100000000000002</v>
       </c>
       <c r="D7" s="1">
-        <v>0.62445816366741103</v>
+        <v>0.624</v>
       </c>
       <c r="E7" s="1">
-        <v>0.67478940157985201</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="F7" s="1">
-        <v>0.10285194174757201</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="G7" s="1">
-        <v>6.8567454798330998E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="H7" s="1">
-        <v>0.68907563025209995</v>
+        <v>0.68899999999999995</v>
       </c>
       <c r="I7" s="1">
-        <v>0.65723495702005696</v>
+        <v>0.65700000000000003</v>
       </c>
       <c r="J7" s="1">
-        <v>0.32127031019202301</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.41900000000000004</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="1"/>
+        <v>subset_6 &amp; 0.496 &amp; 0.651 &amp; 0.624 &amp; 0.675 &amp; 0.103 &amp; 0.069 &amp; 0.689 &amp; 0.657 &amp; 0.321</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>0.49612403100775099</v>
+        <v>0.496</v>
       </c>
       <c r="C8" s="1">
-        <v>0.65189313517338998</v>
+        <v>0.65200000000000002</v>
       </c>
       <c r="D8" s="1">
-        <v>0.62389821784726196</v>
+        <v>0.624</v>
       </c>
       <c r="E8" s="1">
-        <v>0.67563760752552904</v>
+        <v>0.67600000000000005</v>
       </c>
       <c r="F8" s="1">
-        <v>0.102190705331138</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="G8" s="1">
-        <v>6.7077423854917398E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="H8" s="1">
-        <v>0.68706673776611005</v>
+        <v>0.68700000000000006</v>
       </c>
       <c r="I8" s="1">
-        <v>0.661688684663986</v>
+        <v>0.66200000000000003</v>
       </c>
       <c r="J8" s="1">
-        <v>0.32285197704582902</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.41949999999999998</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="1"/>
+        <v>subset_7 &amp; 0.496 &amp; 0.652 &amp; 0.624 &amp; 0.676 &amp; 0.102 &amp; 0.067 &amp; 0.687 &amp; 0.662 &amp; 0.323</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>0.49612403100775099</v>
+        <v>0.496</v>
       </c>
       <c r="C9" s="1">
-        <v>0.65251994989655604</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="D9" s="1">
-        <v>0.62305602859836995</v>
+        <v>0.623</v>
       </c>
       <c r="E9" s="1">
-        <v>0.67679021071696699</v>
+        <v>0.67700000000000005</v>
       </c>
       <c r="F9" s="1">
-        <v>0.10223292469351999</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="G9" s="1">
-        <v>6.73564819420953E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="H9" s="1">
-        <v>0.68542125600375503</v>
+        <v>0.68500000000000005</v>
       </c>
       <c r="I9" s="1">
-        <v>0.66610333172380398</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="J9" s="1">
-        <v>0.32447830862163601</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.42016666666666663</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="1"/>
+        <v>subset_8 &amp; 0.496 &amp; 0.653 &amp; 0.623 &amp; 0.677 &amp; 0.102 &amp; 0.067 &amp; 0.685 &amp; 0.666 &amp; 0.324</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>0.49612403100775099</v>
+        <v>0.496</v>
       </c>
       <c r="C10" s="1">
-        <v>0.65303250181399597</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="D10" s="1">
-        <v>0.620411839767808</v>
+        <v>0.62</v>
       </c>
       <c r="E10" s="1">
-        <v>0.67774905783232298</v>
+        <v>0.67800000000000005</v>
       </c>
       <c r="F10" s="1">
-        <v>9.9679081979966902E-2</v>
+        <v>0.1</v>
       </c>
       <c r="G10" s="1">
-        <v>6.5393669892754303E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="H10" s="1">
-        <v>0.683544303797468</v>
+        <v>0.68400000000000005</v>
       </c>
       <c r="I10" s="1">
-        <v>0.66624816907302697</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="J10" s="1">
-        <v>0.330888100535145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.42066666666666669</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="1"/>
+        <v>subset_9 &amp; 0.496 &amp; 0.653 &amp; 0.62 &amp; 0.678 &amp; 0.1 &amp; 0.065 &amp; 0.684 &amp; 0.666 &amp; 0.331</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>0.50387596899224796</v>
+        <v>0.504</v>
       </c>
       <c r="C11" s="1">
-        <v>0.65358329111073499</v>
+        <v>0.65400000000000003</v>
       </c>
       <c r="D11" s="1">
-        <v>0.61876935202386896</v>
+        <v>0.61899999999999999</v>
       </c>
       <c r="E11" s="1">
-        <v>0.676341750062324</v>
+        <v>0.67600000000000005</v>
       </c>
       <c r="F11" s="1">
-        <v>9.6974466596712106E-2</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="G11" s="1">
-        <v>6.4738185474514598E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="H11" s="1">
-        <v>0.68239475280996198</v>
+        <v>0.68200000000000005</v>
       </c>
       <c r="I11" s="1">
-        <v>0.664468864468864</v>
+        <v>0.66400000000000003</v>
       </c>
       <c r="J11" s="1">
-        <v>0.33329747175900998</v>
-      </c>
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.41950000000000004</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="1"/>
+        <v>subset_10 &amp; 0.504 &amp; 0.654 &amp; 0.619 &amp; 0.676 &amp; 0.097 &amp; 0.065 &amp; 0.682 &amp; 0.664 &amp; 0.333</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="K2:K11">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{626775EE-57E9-4AAD-B414-924D493D30CB}">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="16.08984375" customWidth="1"/>
+    <col min="3" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.36328125" customWidth="1"/>
+    <col min="6" max="11" width="10.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="E2" s="1">
+        <f>SUM(C2:D2)/COUNT(C2:D2)</f>
+        <v>0.62949999999999995</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.161</v>
+      </c>
+      <c r="H2" s="1">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="L2" s="1">
+        <f>SUM(F2:K2)/COUNT(F2:K2)</f>
+        <v>0.37949999999999995</v>
+      </c>
+      <c r="M2" t="str">
+        <f>_xlfn.TEXTJOIN(" &amp; ", FALSE, A2:K2)</f>
+        <v>subset_1 &amp; 0.411 &amp; 0.642 &amp; 0.617 &amp; 0.6295 &amp; 0.599 &amp; 0.161 &amp; 0.037 &amp; 0.562 &amp; 0.59 &amp; 0.328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.434</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E11" si="0">SUM(C3:D3)/COUNT(C3:D3)</f>
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.157</v>
+      </c>
+      <c r="H3" s="1">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.316</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:L10" si="1">SUM(F3:K3)/COUNT(F3:K3)</f>
+        <v>0.379</v>
+      </c>
+      <c r="M3" t="str">
+        <f>_xlfn.TEXTJOIN(" &amp; ", FALSE, A3:K3)</f>
+        <v>subset_2 &amp; 0.434 &amp; 0.649 &amp; 0.615 &amp; 0.632 &amp; 0.598 &amp; 0.157 &amp; 0.044 &amp; 0.584 &amp; 0.575 &amp; 0.316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.442</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.64749999999999996</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.38333333333333336</v>
+      </c>
+      <c r="M4" t="str">
+        <f>_xlfn.TEXTJOIN(" &amp; ", FALSE, A4:K4)</f>
+        <v>subset_3 &amp; 0.442 &amp; 0.658 &amp; 0.637 &amp; 0.6475 &amp; 0.618 &amp; 0.181 &amp; 0.052 &amp; 0.579 &amp; 0.549 &amp; 0.321</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.64450000000000007</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.627</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.627</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.39583333333333343</v>
+      </c>
+      <c r="M5" t="str">
+        <f>_xlfn.TEXTJOIN(" &amp; ", FALSE, A5:K5)</f>
+        <v>subset_4 &amp; 0.465 &amp; 0.655 &amp; 0.634 &amp; 0.6445 &amp; 0.627 &amp; 0.168 &amp; 0.053 &amp; 0.571 &amp; 0.627 &amp; 0.329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.496</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.627</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.63949999999999996</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.629</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.151</v>
+      </c>
+      <c r="H6" s="1">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.39583333333333343</v>
+      </c>
+      <c r="M6" t="str">
+        <f>_xlfn.TEXTJOIN(" &amp; ", FALSE, A6:K6)</f>
+        <v>subset_5 &amp; 0.496 &amp; 0.652 &amp; 0.627 &amp; 0.6395 &amp; 0.629 &amp; 0.151 &amp; 0.053 &amp; 0.565 &amp; 0.635 &amp; 0.342</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.496</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.624</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.63749999999999996</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="H7" s="1">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.39766666666666667</v>
+      </c>
+      <c r="M7" t="str">
+        <f>_xlfn.TEXTJOIN(" &amp; ", FALSE, A7:K7)</f>
+        <v>subset_6 &amp; 0.496 &amp; 0.651 &amp; 0.624 &amp; 0.6375 &amp; 0.633 &amp; 0.139 &amp; 0.057 &amp; 0.56 &amp; 0.646 &amp; 0.351</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.496</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.624</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="H8" s="1">
+        <v>5.5E-2</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.39749999999999996</v>
+      </c>
+      <c r="M8" t="str">
+        <f>_xlfn.TEXTJOIN(" &amp; ", FALSE, A8:K8)</f>
+        <v>subset_7 &amp; 0.496 &amp; 0.652 &amp; 0.624 &amp; 0.638 &amp; 0.634 &amp; 0.133 &amp; 0.055 &amp; 0.557 &amp; 0.653 &amp; 0.353</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.496</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.623</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="H9" s="1">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="L9" s="1">
+        <f>SUM(F9:K9)/COUNT(F9:K9)</f>
+        <v>0.39833333333333337</v>
+      </c>
+      <c r="M9" t="str">
+        <f>_xlfn.TEXTJOIN(" &amp; ", FALSE, A9:K9)</f>
+        <v>subset_8 &amp; 0.496 &amp; 0.653 &amp; 0.623 &amp; 0.638 &amp; 0.636 &amp; 0.131 &amp; 0.056 &amp; 0.555 &amp; 0.657 &amp; 0.355</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.496</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.63650000000000007</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.129</v>
+      </c>
+      <c r="H10" s="1">
+        <v>5.5E-2</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.39916666666666667</v>
+      </c>
+      <c r="M10" t="str">
+        <f>_xlfn.TEXTJOIN(" &amp; ", FALSE, A10:K10)</f>
+        <v>subset_9 &amp; 0.496 &amp; 0.653 &amp; 0.62 &amp; 0.6365 &amp; 0.638 &amp; 0.129 &amp; 0.055 &amp; 0.553 &amp; 0.658 &amp; 0.362</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.504</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.63650000000000007</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.126</v>
+      </c>
+      <c r="H11" s="1">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="L11" s="1">
+        <f>SUM(F11:K11)/COUNT(F11:K11)</f>
+        <v>0.39850000000000002</v>
+      </c>
+      <c r="M11" t="str">
+        <f>_xlfn.TEXTJOIN(" &amp; ", FALSE, A11:K11)</f>
+        <v>subset_10 &amp; 0.504 &amp; 0.654 &amp; 0.619 &amp; 0.6365 &amp; 0.637 &amp; 0.126 &amp; 0.053 &amp; 0.552 &amp; 0.656 &amp; 0.367</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:K11">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C11">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:E11">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L11">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>